<commit_message>
Added keyboard shortcuts for all functionalities to improve ease of use
</commit_message>
<xml_diff>
--- a/FORMAT.xlsx
+++ b/FORMAT.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shri Karthik\Desktop\DIAGRAM-MAPPER\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{647989DE-AA45-451A-8EF0-FC5FE0013D2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80EC428B-6F2F-4934-BDBF-67FC5D5EA633}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1206,6 +1206,109 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="165" fontId="1" fillId="2" borderId="19" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="0" borderId="20" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="22" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="2" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="2" borderId="1" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1231,10 +1334,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="12" fillId="0" borderId="1" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
@@ -1276,105 +1375,6 @@
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="2" borderId="1" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="2" borderId="19" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="6" fillId="0" borderId="20" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="22" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="6" fillId="2" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -7301,7 +7301,7 @@
   </sheetPr>
   <dimension ref="A1:M162"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showWhiteSpace="0" topLeftCell="A19" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" showWhiteSpace="0" topLeftCell="A2" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
       <selection activeCell="K26" sqref="K26:M26"/>
     </sheetView>
   </sheetViews>
@@ -7309,11 +7309,11 @@
   <cols>
     <col min="1" max="1" width="4.6640625" style="4" customWidth="1"/>
     <col min="2" max="2" width="10.6640625" style="4" customWidth="1"/>
-    <col min="3" max="3" width="24.44140625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="45.33203125" style="4" customWidth="1"/>
     <col min="4" max="4" width="14.44140625" style="6" customWidth="1"/>
     <col min="5" max="5" width="10.33203125" style="4" customWidth="1"/>
     <col min="6" max="6" width="10.109375" style="4" customWidth="1"/>
-    <col min="7" max="7" width="15.88671875" style="4" customWidth="1"/>
+    <col min="7" max="7" width="37" style="4" customWidth="1"/>
     <col min="8" max="8" width="18" style="4" customWidth="1"/>
     <col min="9" max="9" width="11.5546875" style="4" customWidth="1"/>
     <col min="10" max="10" width="11.6640625" style="4" customWidth="1"/>
@@ -7330,128 +7330,128 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="1" customFormat="1" ht="57.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="58" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
-      <c r="I1" s="27"/>
-      <c r="J1" s="28"/>
-      <c r="K1" s="23" t="s">
+      <c r="B1" s="59"/>
+      <c r="C1" s="59"/>
+      <c r="D1" s="59"/>
+      <c r="E1" s="59"/>
+      <c r="F1" s="59"/>
+      <c r="G1" s="59"/>
+      <c r="H1" s="59"/>
+      <c r="I1" s="59"/>
+      <c r="J1" s="60"/>
+      <c r="K1" s="55" t="s">
         <v>24</v>
       </c>
-      <c r="L1" s="24"/>
-      <c r="M1" s="25"/>
+      <c r="L1" s="56"/>
+      <c r="M1" s="57"/>
     </row>
     <row r="2" spans="1:13" s="1" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="35" t="s">
+      <c r="A2" s="66" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="36"/>
-      <c r="C2" s="36"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37"/>
+      <c r="B2" s="67"/>
+      <c r="C2" s="67"/>
+      <c r="D2" s="68"/>
+      <c r="E2" s="68"/>
+      <c r="F2" s="68"/>
+      <c r="G2" s="68"/>
       <c r="H2" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="I2" s="38"/>
-      <c r="J2" s="39"/>
-      <c r="K2" s="39"/>
-      <c r="L2" s="39"/>
-      <c r="M2" s="40"/>
+      <c r="I2" s="69"/>
+      <c r="J2" s="70"/>
+      <c r="K2" s="70"/>
+      <c r="L2" s="70"/>
+      <c r="M2" s="71"/>
     </row>
     <row r="3" spans="1:13" s="1" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="41" t="s">
+      <c r="A3" s="72" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="42"/>
-      <c r="C3" s="42"/>
-      <c r="D3" s="43"/>
-      <c r="E3" s="43"/>
-      <c r="F3" s="37"/>
-      <c r="G3" s="37"/>
+      <c r="B3" s="73"/>
+      <c r="C3" s="73"/>
+      <c r="D3" s="74"/>
+      <c r="E3" s="74"/>
+      <c r="F3" s="68"/>
+      <c r="G3" s="68"/>
       <c r="H3" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="I3" s="33"/>
-      <c r="J3" s="33"/>
-      <c r="K3" s="33"/>
-      <c r="L3" s="33"/>
-      <c r="M3" s="34"/>
+      <c r="I3" s="64"/>
+      <c r="J3" s="64"/>
+      <c r="K3" s="64"/>
+      <c r="L3" s="64"/>
+      <c r="M3" s="65"/>
     </row>
     <row r="4" spans="1:13" s="1" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="29" t="s">
+      <c r="A4" s="61" t="s">
         <v>22</v>
       </c>
-      <c r="B4" s="30"/>
-      <c r="C4" s="30"/>
-      <c r="D4" s="31"/>
-      <c r="E4" s="32"/>
-      <c r="F4" s="32"/>
-      <c r="G4" s="32"/>
+      <c r="B4" s="62"/>
+      <c r="C4" s="62"/>
+      <c r="D4" s="63"/>
+      <c r="E4" s="48"/>
+      <c r="F4" s="48"/>
+      <c r="G4" s="48"/>
       <c r="H4" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="I4" s="33"/>
-      <c r="J4" s="33"/>
-      <c r="K4" s="33"/>
-      <c r="L4" s="33"/>
-      <c r="M4" s="34"/>
+      <c r="I4" s="64"/>
+      <c r="J4" s="64"/>
+      <c r="K4" s="64"/>
+      <c r="L4" s="64"/>
+      <c r="M4" s="65"/>
     </row>
     <row r="5" spans="1:13" s="1" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="44" t="s">
+      <c r="A5" s="46" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="45"/>
-      <c r="C5" s="45"/>
-      <c r="D5" s="32"/>
-      <c r="E5" s="32"/>
-      <c r="F5" s="32"/>
-      <c r="G5" s="32"/>
+      <c r="B5" s="47"/>
+      <c r="C5" s="47"/>
+      <c r="D5" s="48"/>
+      <c r="E5" s="48"/>
+      <c r="F5" s="48"/>
+      <c r="G5" s="48"/>
       <c r="H5" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="I5" s="46"/>
-      <c r="J5" s="46"/>
-      <c r="K5" s="46"/>
-      <c r="L5" s="46"/>
-      <c r="M5" s="47"/>
+      <c r="I5" s="49"/>
+      <c r="J5" s="49"/>
+      <c r="K5" s="49"/>
+      <c r="L5" s="49"/>
+      <c r="M5" s="50"/>
     </row>
     <row r="6" spans="1:13" s="1" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="48" t="s">
+      <c r="A6" s="51" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="49"/>
-      <c r="C6" s="49"/>
-      <c r="D6" s="49"/>
-      <c r="E6" s="49"/>
-      <c r="F6" s="49"/>
-      <c r="G6" s="50" t="s">
+      <c r="B6" s="52"/>
+      <c r="C6" s="52"/>
+      <c r="D6" s="52"/>
+      <c r="E6" s="52"/>
+      <c r="F6" s="52"/>
+      <c r="G6" s="53" t="s">
         <v>4</v>
       </c>
-      <c r="H6" s="51" t="s">
+      <c r="H6" s="54" t="s">
         <v>5</v>
       </c>
-      <c r="I6" s="51" t="s">
+      <c r="I6" s="54" t="s">
         <v>6</v>
       </c>
-      <c r="J6" s="51" t="s">
+      <c r="J6" s="54" t="s">
         <v>7</v>
       </c>
-      <c r="K6" s="51" t="s">
+      <c r="K6" s="54" t="s">
         <v>8</v>
       </c>
-      <c r="L6" s="51" t="s">
+      <c r="L6" s="54" t="s">
         <v>9</v>
       </c>
-      <c r="M6" s="55" t="s">
+      <c r="M6" s="32" t="s">
         <v>10</v>
       </c>
     </row>
@@ -7474,13 +7474,13 @@
       <c r="F7" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="G7" s="51"/>
-      <c r="H7" s="51"/>
-      <c r="I7" s="51"/>
-      <c r="J7" s="51"/>
-      <c r="K7" s="51"/>
-      <c r="L7" s="51"/>
-      <c r="M7" s="55"/>
+      <c r="G7" s="54"/>
+      <c r="H7" s="54"/>
+      <c r="I7" s="54"/>
+      <c r="J7" s="54"/>
+      <c r="K7" s="54"/>
+      <c r="L7" s="54"/>
+      <c r="M7" s="32"/>
     </row>
     <row r="8" spans="1:13" s="1" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="17"/>
@@ -7710,74 +7710,74 @@
     <row r="23" spans="1:13" s="1" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="17"/>
       <c r="B23" s="3"/>
-      <c r="C23" s="63"/>
-      <c r="D23" s="66"/>
-      <c r="E23" s="66"/>
-      <c r="F23" s="66"/>
-      <c r="G23" s="67"/>
-      <c r="H23" s="68"/>
-      <c r="I23" s="68"/>
-      <c r="J23" s="68"/>
-      <c r="K23" s="68"/>
-      <c r="L23" s="68"/>
-      <c r="M23" s="69"/>
+      <c r="C23" s="23"/>
+      <c r="D23" s="24"/>
+      <c r="E23" s="24"/>
+      <c r="F23" s="24"/>
+      <c r="G23" s="25"/>
+      <c r="H23" s="26"/>
+      <c r="I23" s="26"/>
+      <c r="J23" s="26"/>
+      <c r="K23" s="26"/>
+      <c r="L23" s="26"/>
+      <c r="M23" s="27"/>
     </row>
     <row r="24" spans="1:13" s="1" customFormat="1" ht="70.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="65" t="s">
+      <c r="A24" s="44" t="s">
         <v>28</v>
       </c>
-      <c r="B24" s="64"/>
-      <c r="C24" s="74" t="s">
+      <c r="B24" s="45"/>
+      <c r="C24" s="42" t="s">
         <v>18</v>
       </c>
-      <c r="D24" s="62"/>
-      <c r="E24" s="62"/>
-      <c r="F24" s="62"/>
-      <c r="G24" s="62"/>
-      <c r="H24" s="62"/>
-      <c r="I24" s="62"/>
-      <c r="J24" s="62"/>
-      <c r="K24" s="62"/>
-      <c r="L24" s="62"/>
-      <c r="M24" s="62"/>
+      <c r="D24" s="43"/>
+      <c r="E24" s="43"/>
+      <c r="F24" s="43"/>
+      <c r="G24" s="43"/>
+      <c r="H24" s="43"/>
+      <c r="I24" s="43"/>
+      <c r="J24" s="43"/>
+      <c r="K24" s="43"/>
+      <c r="L24" s="43"/>
+      <c r="M24" s="43"/>
     </row>
     <row r="25" spans="1:13" s="1" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="21" t="s">
         <v>16</v>
       </c>
       <c r="B25" s="22"/>
-      <c r="C25" s="70"/>
-      <c r="D25" s="71"/>
-      <c r="E25" s="72"/>
-      <c r="F25" s="72"/>
-      <c r="G25" s="72"/>
-      <c r="H25" s="72"/>
-      <c r="I25" s="72"/>
-      <c r="J25" s="72"/>
-      <c r="K25" s="72"/>
-      <c r="L25" s="72"/>
-      <c r="M25" s="73"/>
+      <c r="C25" s="28"/>
+      <c r="D25" s="35"/>
+      <c r="E25" s="36"/>
+      <c r="F25" s="36"/>
+      <c r="G25" s="36"/>
+      <c r="H25" s="36"/>
+      <c r="I25" s="36"/>
+      <c r="J25" s="36"/>
+      <c r="K25" s="36"/>
+      <c r="L25" s="36"/>
+      <c r="M25" s="37"/>
     </row>
     <row r="26" spans="1:13" s="1" customFormat="1" ht="60.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="52" t="s">
+      <c r="A26" s="29" t="s">
         <v>26</v>
       </c>
-      <c r="B26" s="53"/>
-      <c r="C26" s="56"/>
-      <c r="D26" s="57"/>
-      <c r="E26" s="54" t="s">
+      <c r="B26" s="30"/>
+      <c r="C26" s="33"/>
+      <c r="D26" s="34"/>
+      <c r="E26" s="31" t="s">
         <v>29</v>
       </c>
-      <c r="F26" s="53"/>
-      <c r="G26" s="58"/>
-      <c r="H26" s="59"/>
-      <c r="I26" s="58" t="s">
+      <c r="F26" s="30"/>
+      <c r="G26" s="38"/>
+      <c r="H26" s="39"/>
+      <c r="I26" s="38" t="s">
         <v>17</v>
       </c>
-      <c r="J26" s="59"/>
-      <c r="K26" s="58"/>
-      <c r="L26" s="60"/>
-      <c r="M26" s="61"/>
+      <c r="J26" s="39"/>
+      <c r="K26" s="38"/>
+      <c r="L26" s="40"/>
+      <c r="M26" s="41"/>
     </row>
     <row r="27" spans="1:13" s="1" customFormat="1" ht="48.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="4"/>
@@ -8995,26 +8995,6 @@
     </row>
   </sheetData>
   <mergeCells count="31">
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="M6:M7"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="D25:M25"/>
-    <mergeCell ref="G26:H26"/>
-    <mergeCell ref="I26:J26"/>
-    <mergeCell ref="K26:M26"/>
-    <mergeCell ref="C24:M24"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="A5:C5"/>
-    <mergeCell ref="D5:G5"/>
-    <mergeCell ref="I5:M5"/>
-    <mergeCell ref="A6:F6"/>
-    <mergeCell ref="G6:G7"/>
-    <mergeCell ref="H6:H7"/>
-    <mergeCell ref="I6:I7"/>
-    <mergeCell ref="J6:J7"/>
-    <mergeCell ref="K6:K7"/>
-    <mergeCell ref="L6:L7"/>
     <mergeCell ref="K1:M1"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A4:C4"/>
@@ -9026,6 +9006,26 @@
     <mergeCell ref="A3:C3"/>
     <mergeCell ref="D3:G3"/>
     <mergeCell ref="I3:M3"/>
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="D5:G5"/>
+    <mergeCell ref="I5:M5"/>
+    <mergeCell ref="A6:F6"/>
+    <mergeCell ref="G6:G7"/>
+    <mergeCell ref="H6:H7"/>
+    <mergeCell ref="I6:I7"/>
+    <mergeCell ref="J6:J7"/>
+    <mergeCell ref="K6:K7"/>
+    <mergeCell ref="L6:L7"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="M6:M7"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="D25:M25"/>
+    <mergeCell ref="G26:H26"/>
+    <mergeCell ref="I26:J26"/>
+    <mergeCell ref="K26:M26"/>
+    <mergeCell ref="C24:M24"/>
+    <mergeCell ref="A24:B24"/>
   </mergeCells>
   <conditionalFormatting sqref="M8:M23 M27:M97">
     <cfRule type="cellIs" dxfId="3" priority="14" stopIfTrue="1" operator="equal">

</xml_diff>

<commit_message>
started creation of new version for workbyn format, inserted worbyn format file
</commit_message>
<xml_diff>
--- a/FORMAT.xlsx
+++ b/FORMAT.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shri Karthik\Desktop\DIAGRAM-MAPPER\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80EC428B-6F2F-4934-BDBF-67FC5D5EA633}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24DC8DAF-49DB-42ED-A1C0-1B440980BEA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FAIR" sheetId="1" r:id="rId1"/>
@@ -1226,6 +1226,104 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="1" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1278,104 +1376,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="1" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -1487,6 +1487,136 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>761821</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>409128</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>778381</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>426048</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="2" name="Ink 1">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C3F2FCCC-CD83-7146-24DC-C3DEBC4C38CF}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="4926240" y="3669779"/>
+            <a:ext cx="16560" cy="16920"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="2" name="Ink 1">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C3F2FCCC-CD83-7146-24DC-C3DEBC4C38CF}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="4921920" y="3665459"/>
+              <a:ext cx="25200" cy="25560"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>197576</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>79019</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>210536</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>114299</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="4" name="Ink 3">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7BF1BDCD-3035-D796-8743-E79BE522A9B5}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="6754320" y="3889019"/>
+            <a:ext cx="12960" cy="35280"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="4" name="Ink 3">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7BF1BDCD-3035-D796-8743-E79BE522A9B5}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="6750000" y="3884699"/>
+              <a:ext cx="21600" cy="43920"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -4798,9 +4928,7 @@
       <sheetData sheetId="7"/>
       <sheetData sheetId="8">
         <row r="1">
-          <cell r="K1">
-            <v>0</v>
-          </cell>
+          <cell r="K1"/>
           <cell r="L1" t="str">
             <v>LCL</v>
           </cell>
@@ -5023,7 +5151,7 @@
       <sheetData sheetId="1"/>
       <sheetData sheetId="2" refreshError="1"/>
       <sheetData sheetId="3" refreshError="1"/>
-      <sheetData sheetId="4">
+      <sheetData sheetId="4" refreshError="1">
         <row r="21">
           <cell r="C21" t="str">
             <v>Enter Tol.</v>
@@ -7007,6 +7135,68 @@
     </sheetDataSet>
   </externalBook>
 </externalLink>
+</file>
+
+<file path=xl/ink/ink1.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
+          <inkml:channel name="OA" type="integer" max="360" units="deg"/>
+          <inkml:channel name="OE" type="integer" max="90" units="deg"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
+          <inkml:channelProperty channel="OA" name="resolution" value="1000" units="1/deg"/>
+          <inkml:channelProperty channel="OE" name="resolution" value="1000" units="1/deg"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2025-12-30T14:22:07.333"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.025" units="cm"/>
+      <inkml:brushProperty name="height" value="0.025" units="cm"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">46 1 0 0 0,'0'5'188'0'0,"0"0"168"0"0,-9 0-36 0 0,9 0-60 0 0,0 1-68 0 0,-9-1-60 0 0,0 0-68 0 0,9 0-56 0 0,-9-5-56 0 0,9 5-96 0 0,-9-5-432 0 0</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink2.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
+          <inkml:channel name="OA" type="integer" max="360" units="deg"/>
+          <inkml:channel name="OE" type="integer" max="90" units="deg"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
+          <inkml:channelProperty channel="OA" name="resolution" value="1000" units="1/deg"/>
+          <inkml:channelProperty channel="OE" name="resolution" value="1000" units="1/deg"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2025-12-30T14:22:07.644"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.025" units="cm"/>
+      <inkml:brushProperty name="height" value="0.025" units="cm"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">28 97 0 0 0,'8'-4'2848'0'0,"-14"1"-2463"0"0,5 3-366 0 0,1 0 0 0 0,-1 0 1 0 0,1 0-1 0 0,-1 0 1 0 0,1 0-1 0 0,-1-1 0 0 0,1 1 1 0 0,-1 0-1 0 0,1 0 1 0 0,-1-1-1 0 0,1 1 0 0 0,-1 0 1 0 0,1-1-1 0 0,0 1 1 0 0,-1 0-1 0 0,1-1 1 0 0,-1 1-1 0 0,1-1 0 0 0,0 1 1 0 0,0-1-1 0 0,-1 1 1 0 0,1-1-1 0 0,0 1 0 0 0,0-1 1 0 0,-1 1-1 0 0,1-1 1 0 0,0 1-1 0 0,0-1 0 0 0,0 1 1 0 0,0-1-1 0 0,0 1 1 0 0,0-1-1 0 0,-3-4-222 0 0,2 4 172 0 0,1 1 1 0 0,-1-1-1 0 0,1 1 1 0 0,-1 0 0 0 0,1-1-1 0 0,0 1 1 0 0,-1-1 0 0 0,1 1-1 0 0,0-1 1 0 0,-1 1 0 0 0,1-1-1 0 0,0 1 1 0 0,0-1-1 0 0,-1 1 1 0 0,1-1 0 0 0,0 0-1 0 0,0 1 1 0 0,0-1 0 0 0,0 1-1 0 0,0-1 1 0 0,0 0 0 0 0,-9-34-1767 0 0,9 15 731 0 0,0 14 927 0 0</inkml:trace>
+</inkml:ink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -7301,8 +7491,8 @@
   </sheetPr>
   <dimension ref="A1:M162"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showWhiteSpace="0" topLeftCell="A2" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
-      <selection activeCell="K26" sqref="K26:M26"/>
+    <sheetView showGridLines="0" tabSelected="1" showWhiteSpace="0" topLeftCell="A5" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="30.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -7330,128 +7520,128 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="1" customFormat="1" ht="57.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="58" t="s">
+      <c r="A1" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="59"/>
-      <c r="C1" s="59"/>
-      <c r="D1" s="59"/>
-      <c r="E1" s="59"/>
-      <c r="F1" s="59"/>
-      <c r="G1" s="59"/>
-      <c r="H1" s="59"/>
-      <c r="I1" s="59"/>
-      <c r="J1" s="60"/>
-      <c r="K1" s="55" t="s">
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
+      <c r="I1" s="33"/>
+      <c r="J1" s="34"/>
+      <c r="K1" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="L1" s="56"/>
-      <c r="M1" s="57"/>
+      <c r="L1" s="30"/>
+      <c r="M1" s="31"/>
     </row>
     <row r="2" spans="1:13" s="1" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="66" t="s">
+      <c r="A2" s="41" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="67"/>
-      <c r="C2" s="67"/>
-      <c r="D2" s="68"/>
-      <c r="E2" s="68"/>
-      <c r="F2" s="68"/>
-      <c r="G2" s="68"/>
+      <c r="B2" s="42"/>
+      <c r="C2" s="42"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="43"/>
+      <c r="G2" s="43"/>
       <c r="H2" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="I2" s="69"/>
-      <c r="J2" s="70"/>
-      <c r="K2" s="70"/>
-      <c r="L2" s="70"/>
-      <c r="M2" s="71"/>
+      <c r="I2" s="44"/>
+      <c r="J2" s="45"/>
+      <c r="K2" s="45"/>
+      <c r="L2" s="45"/>
+      <c r="M2" s="46"/>
     </row>
     <row r="3" spans="1:13" s="1" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="72" t="s">
+      <c r="A3" s="47" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="73"/>
-      <c r="C3" s="73"/>
-      <c r="D3" s="74"/>
-      <c r="E3" s="74"/>
-      <c r="F3" s="68"/>
-      <c r="G3" s="68"/>
+      <c r="B3" s="48"/>
+      <c r="C3" s="48"/>
+      <c r="D3" s="49"/>
+      <c r="E3" s="49"/>
+      <c r="F3" s="43"/>
+      <c r="G3" s="43"/>
       <c r="H3" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="I3" s="64"/>
-      <c r="J3" s="64"/>
-      <c r="K3" s="64"/>
-      <c r="L3" s="64"/>
-      <c r="M3" s="65"/>
+      <c r="I3" s="39"/>
+      <c r="J3" s="39"/>
+      <c r="K3" s="39"/>
+      <c r="L3" s="39"/>
+      <c r="M3" s="40"/>
     </row>
     <row r="4" spans="1:13" s="1" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="61" t="s">
+      <c r="A4" s="35" t="s">
         <v>22</v>
       </c>
-      <c r="B4" s="62"/>
-      <c r="C4" s="62"/>
-      <c r="D4" s="63"/>
-      <c r="E4" s="48"/>
-      <c r="F4" s="48"/>
-      <c r="G4" s="48"/>
+      <c r="B4" s="36"/>
+      <c r="C4" s="36"/>
+      <c r="D4" s="37"/>
+      <c r="E4" s="38"/>
+      <c r="F4" s="38"/>
+      <c r="G4" s="38"/>
       <c r="H4" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="I4" s="64"/>
-      <c r="J4" s="64"/>
-      <c r="K4" s="64"/>
-      <c r="L4" s="64"/>
-      <c r="M4" s="65"/>
+      <c r="I4" s="39"/>
+      <c r="J4" s="39"/>
+      <c r="K4" s="39"/>
+      <c r="L4" s="39"/>
+      <c r="M4" s="40"/>
     </row>
     <row r="5" spans="1:13" s="1" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="46" t="s">
+      <c r="A5" s="50" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="47"/>
-      <c r="C5" s="47"/>
-      <c r="D5" s="48"/>
-      <c r="E5" s="48"/>
-      <c r="F5" s="48"/>
-      <c r="G5" s="48"/>
+      <c r="B5" s="51"/>
+      <c r="C5" s="51"/>
+      <c r="D5" s="38"/>
+      <c r="E5" s="38"/>
+      <c r="F5" s="38"/>
+      <c r="G5" s="38"/>
       <c r="H5" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="I5" s="49"/>
-      <c r="J5" s="49"/>
-      <c r="K5" s="49"/>
-      <c r="L5" s="49"/>
-      <c r="M5" s="50"/>
+      <c r="I5" s="52"/>
+      <c r="J5" s="52"/>
+      <c r="K5" s="52"/>
+      <c r="L5" s="52"/>
+      <c r="M5" s="53"/>
     </row>
     <row r="6" spans="1:13" s="1" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="51" t="s">
+      <c r="A6" s="54" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="52"/>
-      <c r="C6" s="52"/>
-      <c r="D6" s="52"/>
-      <c r="E6" s="52"/>
-      <c r="F6" s="52"/>
-      <c r="G6" s="53" t="s">
+      <c r="B6" s="55"/>
+      <c r="C6" s="55"/>
+      <c r="D6" s="55"/>
+      <c r="E6" s="55"/>
+      <c r="F6" s="55"/>
+      <c r="G6" s="56" t="s">
         <v>4</v>
       </c>
-      <c r="H6" s="54" t="s">
+      <c r="H6" s="57" t="s">
         <v>5</v>
       </c>
-      <c r="I6" s="54" t="s">
+      <c r="I6" s="57" t="s">
         <v>6</v>
       </c>
-      <c r="J6" s="54" t="s">
+      <c r="J6" s="57" t="s">
         <v>7</v>
       </c>
-      <c r="K6" s="54" t="s">
+      <c r="K6" s="57" t="s">
         <v>8</v>
       </c>
-      <c r="L6" s="54" t="s">
+      <c r="L6" s="57" t="s">
         <v>9</v>
       </c>
-      <c r="M6" s="32" t="s">
+      <c r="M6" s="61" t="s">
         <v>10</v>
       </c>
     </row>
@@ -7474,13 +7664,13 @@
       <c r="F7" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="G7" s="54"/>
-      <c r="H7" s="54"/>
-      <c r="I7" s="54"/>
-      <c r="J7" s="54"/>
-      <c r="K7" s="54"/>
-      <c r="L7" s="54"/>
-      <c r="M7" s="32"/>
+      <c r="G7" s="57"/>
+      <c r="H7" s="57"/>
+      <c r="I7" s="57"/>
+      <c r="J7" s="57"/>
+      <c r="K7" s="57"/>
+      <c r="L7" s="57"/>
+      <c r="M7" s="61"/>
     </row>
     <row r="8" spans="1:13" s="1" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="17"/>
@@ -7723,23 +7913,23 @@
       <c r="M23" s="27"/>
     </row>
     <row r="24" spans="1:13" s="1" customFormat="1" ht="70.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="44" t="s">
+      <c r="A24" s="73" t="s">
         <v>28</v>
       </c>
-      <c r="B24" s="45"/>
-      <c r="C24" s="42" t="s">
+      <c r="B24" s="74"/>
+      <c r="C24" s="71" t="s">
         <v>18</v>
       </c>
-      <c r="D24" s="43"/>
-      <c r="E24" s="43"/>
-      <c r="F24" s="43"/>
-      <c r="G24" s="43"/>
-      <c r="H24" s="43"/>
-      <c r="I24" s="43"/>
-      <c r="J24" s="43"/>
-      <c r="K24" s="43"/>
-      <c r="L24" s="43"/>
-      <c r="M24" s="43"/>
+      <c r="D24" s="72"/>
+      <c r="E24" s="72"/>
+      <c r="F24" s="72"/>
+      <c r="G24" s="72"/>
+      <c r="H24" s="72"/>
+      <c r="I24" s="72"/>
+      <c r="J24" s="72"/>
+      <c r="K24" s="72"/>
+      <c r="L24" s="72"/>
+      <c r="M24" s="72"/>
     </row>
     <row r="25" spans="1:13" s="1" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="21" t="s">
@@ -7747,37 +7937,37 @@
       </c>
       <c r="B25" s="22"/>
       <c r="C25" s="28"/>
-      <c r="D25" s="35"/>
-      <c r="E25" s="36"/>
-      <c r="F25" s="36"/>
-      <c r="G25" s="36"/>
-      <c r="H25" s="36"/>
-      <c r="I25" s="36"/>
-      <c r="J25" s="36"/>
-      <c r="K25" s="36"/>
-      <c r="L25" s="36"/>
-      <c r="M25" s="37"/>
+      <c r="D25" s="64"/>
+      <c r="E25" s="65"/>
+      <c r="F25" s="65"/>
+      <c r="G25" s="65"/>
+      <c r="H25" s="65"/>
+      <c r="I25" s="65"/>
+      <c r="J25" s="65"/>
+      <c r="K25" s="65"/>
+      <c r="L25" s="65"/>
+      <c r="M25" s="66"/>
     </row>
     <row r="26" spans="1:13" s="1" customFormat="1" ht="60.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="29" t="s">
+      <c r="A26" s="58" t="s">
         <v>26</v>
       </c>
-      <c r="B26" s="30"/>
-      <c r="C26" s="33"/>
-      <c r="D26" s="34"/>
-      <c r="E26" s="31" t="s">
+      <c r="B26" s="59"/>
+      <c r="C26" s="62"/>
+      <c r="D26" s="63"/>
+      <c r="E26" s="60" t="s">
         <v>29</v>
       </c>
-      <c r="F26" s="30"/>
-      <c r="G26" s="38"/>
-      <c r="H26" s="39"/>
-      <c r="I26" s="38" t="s">
+      <c r="F26" s="59"/>
+      <c r="G26" s="67"/>
+      <c r="H26" s="68"/>
+      <c r="I26" s="67" t="s">
         <v>17</v>
       </c>
-      <c r="J26" s="39"/>
-      <c r="K26" s="38"/>
-      <c r="L26" s="40"/>
-      <c r="M26" s="41"/>
+      <c r="J26" s="68"/>
+      <c r="K26" s="67"/>
+      <c r="L26" s="69"/>
+      <c r="M26" s="70"/>
     </row>
     <row r="27" spans="1:13" s="1" customFormat="1" ht="48.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="4"/>
@@ -8995,6 +9185,26 @@
     </row>
   </sheetData>
   <mergeCells count="31">
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="M6:M7"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="D25:M25"/>
+    <mergeCell ref="G26:H26"/>
+    <mergeCell ref="I26:J26"/>
+    <mergeCell ref="K26:M26"/>
+    <mergeCell ref="C24:M24"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="D5:G5"/>
+    <mergeCell ref="I5:M5"/>
+    <mergeCell ref="A6:F6"/>
+    <mergeCell ref="G6:G7"/>
+    <mergeCell ref="H6:H7"/>
+    <mergeCell ref="I6:I7"/>
+    <mergeCell ref="J6:J7"/>
+    <mergeCell ref="K6:K7"/>
+    <mergeCell ref="L6:L7"/>
     <mergeCell ref="K1:M1"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A4:C4"/>
@@ -9006,26 +9216,6 @@
     <mergeCell ref="A3:C3"/>
     <mergeCell ref="D3:G3"/>
     <mergeCell ref="I3:M3"/>
-    <mergeCell ref="A5:C5"/>
-    <mergeCell ref="D5:G5"/>
-    <mergeCell ref="I5:M5"/>
-    <mergeCell ref="A6:F6"/>
-    <mergeCell ref="G6:G7"/>
-    <mergeCell ref="H6:H7"/>
-    <mergeCell ref="I6:I7"/>
-    <mergeCell ref="J6:J7"/>
-    <mergeCell ref="K6:K7"/>
-    <mergeCell ref="L6:L7"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="M6:M7"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="D25:M25"/>
-    <mergeCell ref="G26:H26"/>
-    <mergeCell ref="I26:J26"/>
-    <mergeCell ref="K26:M26"/>
-    <mergeCell ref="C24:M24"/>
-    <mergeCell ref="A24:B24"/>
   </mergeCells>
   <conditionalFormatting sqref="M8:M23 M27:M97">
     <cfRule type="cellIs" dxfId="3" priority="14" stopIfTrue="1" operator="equal">

</xml_diff>